<commit_message>
updated data, fixed some bugs, and added figures
</commit_message>
<xml_diff>
--- a/bond_prices_chosen_bonds.xlsx
+++ b/bond_prices_chosen_bonds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Mathematics\Finance\apm466_assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF893DC-C3E8-4E2B-9334-3148FE220A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0325A2-C720-44EF-8A11-B6A8CFE1DE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6990" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="9" xr2:uid="{0F7BA7DB-B00E-4516-B71B-EEC1447E3BE9}"/>
+    <workbookView xWindow="-28800" yWindow="7275" windowWidth="28800" windowHeight="15435" xr2:uid="{0F7BA7DB-B00E-4516-B71B-EEC1447E3BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="January 6" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46329F1-938D-40B8-AB36-5C1219D82186}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,20 +539,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.41</v>
+        <v>99.73</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-06", E2)</f>
-        <v>0.40277777777777779</v>
+        <f>ROUND(YEARFRAC("2025-01-06", E2), 4)</f>
+        <v>0.15279999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -563,20 +563,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>100</v>
+        <v>98.4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-06", E3)</f>
-        <v>0.73611111111111116</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-06", E3), 4)</f>
+        <v>0.65280000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,7 +600,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1527777777777777</v>
+        <v>1.1528</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6527777777777777</v>
+        <v>1.6528</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -648,7 +648,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1527777777777777</v>
+        <v>2.1528</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -672,7 +672,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6527777777777777</v>
+        <v>2.6528</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -696,7 +696,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1527777777777777</v>
+        <v>3.1528</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -720,7 +720,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6527777777777777</v>
+        <v>3.6528</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -744,7 +744,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1527777777777777</v>
+        <v>4.1528</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -768,7 +768,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6527777777777777</v>
+        <v>4.6528</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,22 +792,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1527777777777777</v>
+        <v>5.1528</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{83B1B519-529C-4404-A2FD-19D6C1D26DCD}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{85CDA569-9455-4EBA-B0B9-2458D19CFC1C}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{DBD9E49B-5D7F-415F-AD28-8F56F450F995}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{ED2F4F61-4B46-4ED5-A494-467E8EA97E30}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{4D1BAB16-D8CE-46BB-B8C5-AC0A1B46546D}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{42C9FD66-326A-4829-BCB2-E075C2B9F939}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{D72723FE-3B6A-414B-8DCC-94477DDFAD2B}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{44B12221-1F52-47F9-93EC-82CB8974306C}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{091C8D82-DA17-4055-AE5E-10FDE75B5960}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{35821779-847A-462C-91A0-ECD21E979EE9}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{0EE11BAD-AE57-4FCE-86C9-CBFC9614AA06}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{DBD9E49B-5D7F-415F-AD28-8F56F450F995}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{ED2F4F61-4B46-4ED5-A494-467E8EA97E30}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{4D1BAB16-D8CE-46BB-B8C5-AC0A1B46546D}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{42C9FD66-326A-4829-BCB2-E075C2B9F939}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{D72723FE-3B6A-414B-8DCC-94477DDFAD2B}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{44B12221-1F52-47F9-93EC-82CB8974306C}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{091C8D82-DA17-4055-AE5E-10FDE75B5960}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{35821779-847A-462C-91A0-ECD21E979EE9}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{0EE11BAD-AE57-4FCE-86C9-CBFC9614AA06}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{F5A8CAEC-E041-4D78-A73E-900F14A5DFF3}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{11BA9E19-D533-4427-9DFF-A166B75848F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EA36FF-4DDE-45B9-A793-EC02DDBA74C7}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,20 +857,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.17</v>
+        <v>99.8</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-17", E2)</f>
-        <v>0.37222222222222223</v>
+        <f>ROUND(YEARFRAC("2025-01-17", E2), 4)</f>
+        <v>0.1222</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -881,20 +881,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>100.01</v>
+        <v>98.5</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-17", E3)</f>
-        <v>0.7055555555555556</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-17", E3), 4)</f>
+        <v>0.62219999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -914,11 +914,11 @@
         <v>46082</v>
       </c>
       <c r="F4" s="2">
-        <v>96.31</v>
+        <v>97.06</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1222222222222222</v>
+        <v>1.1222000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -938,11 +938,11 @@
         <v>46266</v>
       </c>
       <c r="F5" s="2">
-        <v>96.36</v>
+        <v>97.07</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6222222222222222</v>
+        <v>1.6222000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -966,7 +966,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1222222222222222</v>
+        <v>2.1221999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6222222222222222</v>
+        <v>2.6221999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1014,7 +1014,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1222222222222222</v>
+        <v>3.1221999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6222222222222222</v>
+        <v>3.6221999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1222222222222218</v>
+        <v>4.1222000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1082,11 +1082,11 @@
         <v>47362</v>
       </c>
       <c r="F11" s="2">
-        <v>103.01</v>
+        <v>101.97</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6222222222222218</v>
+        <v>4.6222000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1110,24 +1110,25 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1222222222222218</v>
+        <v>5.1222000000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{C0C7002F-0504-4CFD-9F66-139C723BFAA2}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{7C0056CC-204E-4797-A81F-73E9D49A3D1E}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{2620D626-CA1B-49E9-8622-B395241E3C0C}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{9912C61B-ED66-4B78-A662-843F1D81ECCA}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{A4E8F1FA-F02D-4F0F-9C3F-C4E40D715CFE}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{A75AFEAE-8E57-40D9-803D-33A6EEA1DCF0}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{C1BFFDFD-A570-4463-97A9-1E4E8343C47D}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{F54B58A0-192F-4A16-AAF2-98563961A6DE}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FF7247B6-D86E-41BB-9C50-D86B851FB016}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{778F6C08-2B63-4F77-A046-428949F968DE}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{6788BF09-8B40-4429-9727-68DD4E839598}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{2620D626-CA1B-49E9-8622-B395241E3C0C}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{9912C61B-ED66-4B78-A662-843F1D81ECCA}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{A4E8F1FA-F02D-4F0F-9C3F-C4E40D715CFE}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{A75AFEAE-8E57-40D9-803D-33A6EEA1DCF0}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{C1BFFDFD-A570-4463-97A9-1E4E8343C47D}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{F54B58A0-192F-4A16-AAF2-98563961A6DE}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FF7247B6-D86E-41BB-9C50-D86B851FB016}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{778F6C08-2B63-4F77-A046-428949F968DE}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{6788BF09-8B40-4429-9727-68DD4E839598}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{86CFC057-7AA1-4659-A80A-ACDDED27C250}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{166DD1DF-FF9C-4A4C-A2B9-D7B2CEBC7C41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -1136,7 +1137,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,20 +1176,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.31</v>
+        <v>99.73</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-07", E2)</f>
-        <v>0.4</v>
+        <f>ROUND(YEARFRAC("2025-01-07", E2), 4)</f>
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1199,20 +1200,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.98</v>
+        <v>98.41</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-07", E3)</f>
-        <v>0.73333333333333328</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-07", E3), 4)</f>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1433,17 +1434,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{6A4583BC-8874-47F2-9D33-0FEE0F80BD08}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{AACE9DE2-17D7-4EFE-9ECE-DE580E1C2AC7}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{1588FA4B-D676-4110-BBC5-6C669A20415D}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{2049C429-CAE6-4A41-8A3F-FEA07991A205}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{20FC8514-A142-49F0-9AB3-506B2E3EEE2E}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{2E737FDB-EE98-4C54-8FE0-EA398AA20BC5}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{B1EC346A-888C-4D92-8DA7-0FC47D00BA67}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{E45C6554-8D56-4AF5-8DF4-693D606D5A84}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{2B152BEC-AA9E-4362-B679-54918C209390}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{C5121767-6A0C-4F3B-B9DC-A866D5012552}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{65B21C2A-B74B-4BFE-9955-D2DCF7048845}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{1588FA4B-D676-4110-BBC5-6C669A20415D}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{2049C429-CAE6-4A41-8A3F-FEA07991A205}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{20FC8514-A142-49F0-9AB3-506B2E3EEE2E}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{2E737FDB-EE98-4C54-8FE0-EA398AA20BC5}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{B1EC346A-888C-4D92-8DA7-0FC47D00BA67}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{E45C6554-8D56-4AF5-8DF4-693D606D5A84}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{2B152BEC-AA9E-4362-B679-54918C209390}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{C5121767-6A0C-4F3B-B9DC-A866D5012552}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{65B21C2A-B74B-4BFE-9955-D2DCF7048845}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{C0328194-2303-4004-BCF9-B2791983FD38}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{F0EA0867-40CB-484B-A212-EEE84FA83CA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1493,20 +1494,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.37</v>
+        <v>99.74</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-08", E2)</f>
-        <v>0.3972222222222222</v>
+        <f>ROUND(YEARFRAC("2025-01-08", E2), 4)</f>
+        <v>0.1472</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1517,20 +1518,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.98</v>
+        <v>98.4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-08", E3)</f>
-        <v>0.73055555555555551</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-08", E3), 4)</f>
+        <v>0.6472</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1554,7 +1555,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1472222222222221</v>
+        <v>1.1472</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1578,7 +1579,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6472222222222221</v>
+        <v>1.6472</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1602,7 +1603,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1472222222222221</v>
+        <v>2.1472000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1626,7 +1627,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6472222222222221</v>
+        <v>2.6472000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1650,7 +1651,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1472222222222221</v>
+        <v>3.1472000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1674,7 +1675,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6472222222222221</v>
+        <v>3.6472000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1698,7 +1699,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1472222222222221</v>
+        <v>4.1471999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1722,7 +1723,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6472222222222221</v>
+        <v>4.6471999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1746,22 +1747,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1472222222222221</v>
+        <v>5.1471999999999998</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{F84462FA-7A55-41B9-8FF3-1B8147BFDF85}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{496585ED-2C69-48C2-BC03-CB0A04A5D46E}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{445961B6-CDDC-477E-850C-26182B14D4F3}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{CEB9A895-E8E9-474D-933C-5C39D2BDEB91}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{0ECA1E5C-BA02-40A8-82F1-E1CB7DD14AFF}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{7EAABCE2-3D3E-4499-8C5B-8C1F5DF2DDD3}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{D92FBF94-9D54-4AA4-AA05-4DA78899AE48}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{83B900A8-CBA8-4E0A-B292-5990926ACFBC}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FA486365-871B-469B-A40F-340D0D6CBD39}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{7B0C08C5-8D1A-4DEB-8C8D-59E969A3495C}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{FFBC6A39-7BB0-4CE9-8C31-76C60AE82D11}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{445961B6-CDDC-477E-850C-26182B14D4F3}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{CEB9A895-E8E9-474D-933C-5C39D2BDEB91}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{0ECA1E5C-BA02-40A8-82F1-E1CB7DD14AFF}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{7EAABCE2-3D3E-4499-8C5B-8C1F5DF2DDD3}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{D92FBF94-9D54-4AA4-AA05-4DA78899AE48}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{83B900A8-CBA8-4E0A-B292-5990926ACFBC}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FA486365-871B-469B-A40F-340D0D6CBD39}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{7B0C08C5-8D1A-4DEB-8C8D-59E969A3495C}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{FFBC6A39-7BB0-4CE9-8C31-76C60AE82D11}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{2602CCDE-FC00-4586-BB65-F0D095F9EF9A}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{CF36C5CC-C239-4BE9-81DF-DA01DE841632}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1811,20 +1812,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.27</v>
+        <v>99.73</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-09", E2)</f>
-        <v>0.39444444444444443</v>
+        <f>ROUND(YEARFRAC("2025-01-09", E2), 4)</f>
+        <v>0.1444</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1835,20 +1836,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.99</v>
+        <v>98.42</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-09", E3)</f>
-        <v>0.72777777777777775</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-09", E3), 4)</f>
+        <v>0.64439999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1872,7 +1873,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1444444444444444</v>
+        <v>1.1444000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1896,7 +1897,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6444444444444444</v>
+        <v>1.6444000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1920,7 +1921,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1444444444444444</v>
+        <v>2.1444000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1944,7 +1945,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6444444444444444</v>
+        <v>2.6444000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1968,7 +1969,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1444444444444444</v>
+        <v>3.1444000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1992,7 +1993,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6444444444444444</v>
+        <v>3.6444000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2016,7 +2017,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1444444444444448</v>
+        <v>4.1444000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2040,7 +2041,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6444444444444448</v>
+        <v>4.6444000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2064,22 +2065,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1444444444444448</v>
+        <v>5.1444000000000001</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{BB58B4C0-E634-46B7-9CB9-D8B7FA71363D}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{E2D92B87-A062-4985-A8F2-9F36F4D3C874}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{CCF26B9F-EA16-46E8-B5F5-03040B43888F}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{105632FD-D198-45B8-AE6C-B0CF1633D96B}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{FBCC395D-0C26-4651-ACFE-6B21D66591CC}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{12CB0D6E-8A4E-4C92-A0D1-2B843B89E8E7}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{86C2DF0F-FEC8-4755-AD7D-6700F541F6DC}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{DFFF189C-FA11-4BCF-BC49-29B5F311EDF6}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{0948F54A-0FCD-4873-9A76-2A10F2EA7367}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{F7FDC09D-147F-460E-A0D2-2CA977E1B94D}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{66569AEE-2195-46F1-8C3C-17009F4675DD}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{CCF26B9F-EA16-46E8-B5F5-03040B43888F}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{105632FD-D198-45B8-AE6C-B0CF1633D96B}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{FBCC395D-0C26-4651-ACFE-6B21D66591CC}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{12CB0D6E-8A4E-4C92-A0D1-2B843B89E8E7}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{86C2DF0F-FEC8-4755-AD7D-6700F541F6DC}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{DFFF189C-FA11-4BCF-BC49-29B5F311EDF6}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{0948F54A-0FCD-4873-9A76-2A10F2EA7367}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{F7FDC09D-147F-460E-A0D2-2CA977E1B94D}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{66569AEE-2195-46F1-8C3C-17009F4675DD}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{888A702B-7F91-44A6-9A13-79AB82B330A4}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{9F706B41-40CA-4462-8EE0-878F25DA45AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2129,20 +2130,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.25</v>
+        <v>99.74</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-10", E2)</f>
-        <v>0.39166666666666666</v>
+        <f>ROUND(YEARFRAC("2025-01-10", E2), 4)</f>
+        <v>0.14169999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2153,20 +2154,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.91</v>
+        <v>98.37</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-10", E3)</f>
-        <v>0.72499999999999998</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-10", E3), 4)</f>
+        <v>0.64170000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2190,7 +2191,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1416666666666666</v>
+        <v>1.1416999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2214,7 +2215,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6416666666666666</v>
+        <v>1.6416999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2238,7 +2239,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1416666666666666</v>
+        <v>2.1417000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2262,7 +2263,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6416666666666666</v>
+        <v>2.6417000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2286,7 +2287,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1416666666666666</v>
+        <v>3.1417000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2310,7 +2311,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6416666666666666</v>
+        <v>3.6417000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2334,7 +2335,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1416666666666666</v>
+        <v>4.1417000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2358,7 +2359,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6416666666666666</v>
+        <v>4.6417000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2382,22 +2383,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1416666666666666</v>
+        <v>5.1417000000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{59C43AD3-3E11-4A47-9038-E9875EDCEAF0}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{28BF47AC-5C39-4B11-8F13-AD3456801B5D}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{2A18690E-0BCC-406C-A37C-616EBF8D846C}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{DCBA4A96-BB6E-44EF-BAB5-35803FB12B0B}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{D67C5328-BF99-41DB-995B-5743D09D83A1}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{60B58878-8DAC-42FD-AE10-4DA49BE7569C}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{BDE0CA30-4E14-4DC7-A052-BEAF66AFCB27}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{BC5FE2FD-BEA3-4156-926A-DF5745B4B735}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{39BD8D42-6E0E-4EDC-B59C-5B000937A8DC}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{68AEF07E-6494-43A2-9B2E-A670DD003784}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{DD9F3FCE-12BB-4ED3-AF3A-FB1B33D959AA}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{2A18690E-0BCC-406C-A37C-616EBF8D846C}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{DCBA4A96-BB6E-44EF-BAB5-35803FB12B0B}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{D67C5328-BF99-41DB-995B-5743D09D83A1}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{60B58878-8DAC-42FD-AE10-4DA49BE7569C}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{BDE0CA30-4E14-4DC7-A052-BEAF66AFCB27}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{BC5FE2FD-BEA3-4156-926A-DF5745B4B735}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{39BD8D42-6E0E-4EDC-B59C-5B000937A8DC}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{68AEF07E-6494-43A2-9B2E-A670DD003784}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{DD9F3FCE-12BB-4ED3-AF3A-FB1B33D959AA}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{5E3FA77A-3C74-4D3D-A32E-7D5AA3C24A94}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{113A9A64-93D1-48A1-8317-E9D1892A14E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2447,20 +2448,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
-      </c>
-      <c r="F2" s="2">
-        <v>102.16</v>
+        <v>45717</v>
+      </c>
+      <c r="F2">
+        <v>99.73</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-13", E2)</f>
-        <v>0.38333333333333336</v>
+        <f>ROUND(YEARFRAC("2025-01-13", E2), 4)</f>
+        <v>0.1333</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2471,20 +2472,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.88</v>
+        <v>98.36</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-13", E3)</f>
-        <v>0.71666666666666667</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-13", E3), 4)</f>
+        <v>0.63329999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2508,7 +2509,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1333333333333333</v>
+        <v>1.1333</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2532,7 +2533,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6333333333333333</v>
+        <v>1.6333</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2556,7 +2557,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1333333333333333</v>
+        <v>2.1333000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2580,7 +2581,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6333333333333333</v>
+        <v>2.6333000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2604,7 +2605,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1333333333333333</v>
+        <v>3.1333000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2628,7 +2629,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6333333333333333</v>
+        <v>3.6333000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2652,7 +2653,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1333333333333337</v>
+        <v>4.1333000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2676,7 +2677,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6333333333333337</v>
+        <v>4.6333000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2700,22 +2701,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1333333333333337</v>
+        <v>5.1333000000000002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{575A9DE6-2567-49A0-9021-D4AF352222BD}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{9BE45F80-5896-4825-BE70-87559EB12E3B}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{0FECF024-A495-471F-AAB2-265CAEB671B2}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{540F1140-86A0-4A29-9A16-3143925F337A}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{0BC8C1E3-10DE-4082-A949-67A8B7D27FB5}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{D11C7811-D597-4B05-A984-58B615D6CD6B}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{4E1EB5C0-8B28-418B-9A20-B9EB7CA2FDA6}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{6EB1206D-8479-45D1-A393-163C0EC70467}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FAAB725D-E1A7-4332-B86C-217A11DAA68E}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{32E0F0F5-2CD7-49CC-9E77-ED9E9A204AC6}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{F2A42D5C-6868-4EF2-A843-2DDB1DC80C5E}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{0FECF024-A495-471F-AAB2-265CAEB671B2}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{540F1140-86A0-4A29-9A16-3143925F337A}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{0BC8C1E3-10DE-4082-A949-67A8B7D27FB5}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{D11C7811-D597-4B05-A984-58B615D6CD6B}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{4E1EB5C0-8B28-418B-9A20-B9EB7CA2FDA6}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{6EB1206D-8479-45D1-A393-163C0EC70467}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{FAAB725D-E1A7-4332-B86C-217A11DAA68E}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{32E0F0F5-2CD7-49CC-9E77-ED9E9A204AC6}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{F2A42D5C-6868-4EF2-A843-2DDB1DC80C5E}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{6A8E67D4-E3D7-4E97-83CE-80B5C2E34EFB}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{061D0232-2A8A-4391-8113-377F05687619}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2726,7 +2727,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,20 +2766,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.14</v>
+        <v>99.73</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-14", E2)</f>
-        <v>0.38055555555555554</v>
+        <f>ROUND(YEARFRAC("2025-01-14", E2), 4)</f>
+        <v>0.13059999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2789,20 +2790,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.86</v>
+        <v>98.36</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-14", E3)</f>
-        <v>0.71388888888888891</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-14", E3), 4)</f>
+        <v>0.63060000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2826,7 +2827,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1305555555555555</v>
+        <v>1.1306</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2850,7 +2851,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6305555555555555</v>
+        <v>1.6306</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2874,7 +2875,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1305555555555555</v>
+        <v>2.1305999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2898,7 +2899,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6305555555555555</v>
+        <v>2.6305999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2922,7 +2923,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1305555555555555</v>
+        <v>3.1305999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2946,7 +2947,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6305555555555555</v>
+        <v>3.6305999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2970,7 +2971,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1305555555555555</v>
+        <v>4.1306000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2994,7 +2995,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6305555555555555</v>
+        <v>4.6306000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3018,22 +3019,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1305555555555555</v>
+        <v>5.1306000000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{6E4365BB-9E08-4E0D-AB56-8DB9D9D4C829}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{04B73E07-D618-47AE-8265-A24AB5F0F8A9}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{32ED2D93-A957-4A57-9666-84D603F9DEF4}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{6E4E0284-773D-4BFC-B659-C618B28470F2}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{CD56D3ED-1D91-4C48-995E-4D2549D26CC1}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{C0FFBB16-E8FB-4AE3-A8A1-2F6AE19D0BC1}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{F89E5F87-BF94-4387-8C8C-C697E43F63AD}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{5ABE893C-548C-4295-86CC-B9D68FC00D6D}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{6F614240-759D-4B52-ACE1-A223A6214E85}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{4D922DF1-97C2-47FA-B2EC-2492C0A6AEAC}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{9743B9F8-B56F-413F-AB41-FFF22A264320}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{32ED2D93-A957-4A57-9666-84D603F9DEF4}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{6E4E0284-773D-4BFC-B659-C618B28470F2}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{CD56D3ED-1D91-4C48-995E-4D2549D26CC1}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{C0FFBB16-E8FB-4AE3-A8A1-2F6AE19D0BC1}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{F89E5F87-BF94-4387-8C8C-C697E43F63AD}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{5ABE893C-548C-4295-86CC-B9D68FC00D6D}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{6F614240-759D-4B52-ACE1-A223A6214E85}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{4D922DF1-97C2-47FA-B2EC-2492C0A6AEAC}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{9743B9F8-B56F-413F-AB41-FFF22A264320}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{5157E5B7-CAD2-4AA4-A41E-8436B1FED879}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{E3DC983B-65EB-4565-AD2F-9454C79B4ABF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3083,20 +3084,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.14</v>
+        <v>99.77</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-15", E2)</f>
-        <v>0.37777777777777777</v>
+        <f>ROUND(YEARFRAC("2025-01-15", E2), 4)</f>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3107,20 +3108,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>99.91</v>
+        <v>98.4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-15", E3)</f>
-        <v>0.71111111111111114</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-15", E3), 4)</f>
+        <v>0.62780000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3144,7 +3145,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>1.1277777777777778</v>
+        <v>1.1277999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3168,7 +3169,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>1.6277777777777778</v>
+        <v>1.6277999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3192,7 +3193,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2.1277777777777778</v>
+        <v>2.1278000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3216,7 +3217,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.6277777777777778</v>
+        <v>2.6278000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3240,7 +3241,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>3.1277777777777778</v>
+        <v>3.1278000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3264,7 +3265,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>3.6277777777777778</v>
+        <v>3.6278000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3288,7 +3289,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>4.1277777777777782</v>
+        <v>4.1277999999999997</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3312,7 +3313,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.6277777777777782</v>
+        <v>4.6277999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3336,22 +3337,22 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>5.1277777777777782</v>
+        <v>5.1277999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{B4BB2754-285B-42BF-A587-14F179B5799A}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{4376E5FE-73B6-45DF-B6F3-048DEF456EB3}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{9826D675-C384-4896-86BE-8EA87742608A}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{9AD6DE07-C448-4A7A-BB06-4CA54E5FCE96}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{F775340F-597A-432F-933D-85B40A1B5A50}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{8B083503-7262-4B4B-B6FB-C367567A29C6}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{6A515BD4-C66E-4167-838D-138C2EF58FB3}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{0461DADC-DD8A-4D79-98E0-20038ADA44E7}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{A840D7E3-C460-483C-A6A6-71C6C9BD2B8E}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{9273F621-0197-4A51-8F19-F092CCD7F1D1}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{DFB2CF37-5109-4E12-9407-92C83BED1427}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{9826D675-C384-4896-86BE-8EA87742608A}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{9AD6DE07-C448-4A7A-BB06-4CA54E5FCE96}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{F775340F-597A-432F-933D-85B40A1B5A50}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{8B083503-7262-4B4B-B6FB-C367567A29C6}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{6A515BD4-C66E-4167-838D-138C2EF58FB3}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{0461DADC-DD8A-4D79-98E0-20038ADA44E7}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{A840D7E3-C460-483C-A6A6-71C6C9BD2B8E}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{9273F621-0197-4A51-8F19-F092CCD7F1D1}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{DFB2CF37-5109-4E12-9407-92C83BED1427}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{3F721161-2ED3-4002-B03D-6C327B56206B}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{6551B44F-B58D-4218-B1FA-4199167C94C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3362,7 +3363,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,20 +3402,20 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
-        <v>0.09</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="D2" s="3">
-        <v>3.0099999999999998E-2</v>
+        <v>3.1099999999999999E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>45809</v>
+        <v>45717</v>
       </c>
       <c r="F2" s="2">
-        <v>102.17</v>
+        <v>99.78</v>
       </c>
       <c r="G2">
-        <f>YEARFRAC("2025-01-16", E2)</f>
-        <v>0.375</v>
+        <f>ROUND(YEARFRAC("2025-01-16", E2), 4)</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3425,20 +3426,20 @@
         <v>7</v>
       </c>
       <c r="C3" s="3">
-        <v>0.03</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="3">
         <v>0.03</v>
       </c>
       <c r="E3" s="4">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="F3" s="2">
-        <v>100</v>
+        <v>98.47</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G12" si="0">YEARFRAC("2025-01-16", E3)</f>
-        <v>0.70833333333333337</v>
+        <f t="shared" ref="G3:G12" si="0">ROUND(YEARFRAC("2025-01-16", E3), 4)</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3659,17 +3660,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{912A4F35-9A77-4531-9088-49B714B8BBBE}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://markets.businessinsider.com/bonds/9_000-canada-government-of-Bond-2025-ca135087vh40" xr:uid="{8B97D511-1504-4108-B8E9-B1C507EA61B8}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{29DA84AE-6FCF-476B-A424-5AD98758CFB2}"/>
-    <hyperlink ref="A9" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{68583AD1-057F-4317-8C66-7154BA45FCB5}"/>
-    <hyperlink ref="A10" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{8D41EABC-4029-4CEC-AFE0-33688FECB104}"/>
-    <hyperlink ref="A11" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{8734E9FD-C943-490D-9772-9566B202AC88}"/>
-    <hyperlink ref="A12" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{6641AF3D-EEF0-4223-8A3C-7F7DA1CDB346}"/>
-    <hyperlink ref="A6" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{E6E51E52-D923-49AC-BA1A-601E8AAA73B2}"/>
-    <hyperlink ref="A7" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{DF406FCC-B1E5-4146-BB88-9351834397DF}"/>
-    <hyperlink ref="A4" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{A83A1437-FD3D-477D-84B4-027AD6B79F9E}"/>
-    <hyperlink ref="A5" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{3DC82053-A09B-4031-970D-DAD496FFEC80}"/>
+    <hyperlink ref="A8" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{29DA84AE-6FCF-476B-A424-5AD98758CFB2}"/>
+    <hyperlink ref="A9" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{68583AD1-057F-4317-8C66-7154BA45FCB5}"/>
+    <hyperlink ref="A10" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{8D41EABC-4029-4CEC-AFE0-33688FECB104}"/>
+    <hyperlink ref="A11" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{8734E9FD-C943-490D-9772-9566B202AC88}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{6641AF3D-EEF0-4223-8A3C-7F7DA1CDB346}"/>
+    <hyperlink ref="A6" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{E6E51E52-D923-49AC-BA1A-601E8AAA73B2}"/>
+    <hyperlink ref="A7" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{DF406FCC-B1E5-4146-BB88-9351834397DF}"/>
+    <hyperlink ref="A4" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{A83A1437-FD3D-477D-84B4-027AD6B79F9E}"/>
+    <hyperlink ref="A5" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{3DC82053-A09B-4031-970D-DAD496FFEC80}"/>
+    <hyperlink ref="A3" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{10D21036-E01B-4861-AFD5-2B08512DD511}"/>
+    <hyperlink ref="A2" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{F1F525DA-3A46-4617-B8DB-5D6D004BAA54}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>